<commit_message>
some changes about JRAQ test
</commit_message>
<xml_diff>
--- a/scoring/forms/JRAQ/JRAQ_test_2.xlsx
+++ b/scoring/forms/JRAQ/JRAQ_test_2.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="question_answers" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="outputs" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="outputs1" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1088,64 +1089,82 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>first_scoring_religious_adherence</t>
+          <t>raw_3_first_scoring_</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>second_scoring_religious_adherence</t>
+          <t>raw_3_second_scoring_</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>38</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>first_scoring_Religious_disobedience</t>
+          <t>first_scoring_religious_adherence</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>second_scoring_Religious_disobedience</t>
+          <t>second_scoring_religious_adherence</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>25</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>raw_3_first_scoring_</t>
+          <t>first_scoring_Religious_disobedience</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>14.16783216783217</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>raw_3_second_scoring_</t>
+          <t>second_scoring_Religious_disobedience</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>38.07030303030303</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>